<commit_message>
Revisada a tabela de aprovadores PCP fabricados.
</commit_message>
<xml_diff>
--- a/_extrafiles/APROVADORES_PCP.xlsx
+++ b/_extrafiles/APROVADORES_PCP.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="41">
   <si>
     <t>CIRINA77</t>
   </si>
@@ -35,12 +35,6 @@
     <t>ELTOBORG</t>
   </si>
   <si>
-    <t>ERIKBARB</t>
-  </si>
-  <si>
-    <t>CARLSOUS</t>
-  </si>
-  <si>
     <t>VWL</t>
   </si>
   <si>
@@ -156,9 +150,6 @@
   </si>
   <si>
     <t>Elton</t>
-  </si>
-  <si>
-    <t>Erik</t>
   </si>
 </sst>
 </file>
@@ -174,7 +165,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -193,12 +184,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -212,11 +197,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -500,7 +484,7 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:D11"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -511,282 +495,282 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" t="s">
         <v>37</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>38</v>
-      </c>
-      <c r="C1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D1" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" s="2" t="s">
+      <c r="A11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>42</v>
+      <c r="C13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>43</v>
+      <c r="A20" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>